<commit_message>
Pushing BOM updates for FlatPack
</commit_message>
<xml_diff>
--- a/REV 0-2 PCB/FlatPack 0-2/FlatPack 0-2 BOM.xlsx
+++ b/REV 0-2 PCB/FlatPack 0-2/FlatPack 0-2 BOM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="299">
   <si>
     <t>Value</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>On Hand</t>
+  </si>
+  <si>
+    <t>BQ7693002</t>
   </si>
 </sst>
 </file>
@@ -1529,18 +1532,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="43" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="43" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1605,6 +1596,18 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1652,23 +1655,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1955,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2003,1493 +1990,1493 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="37">
-        <v>1</v>
-      </c>
-      <c r="C2" s="38">
+      <c r="B2" s="33">
+        <v>1</v>
+      </c>
+      <c r="C2" s="34">
         <v>0.59</v>
       </c>
-      <c r="D2" s="38">
-        <f>B2*C2</f>
+      <c r="D2" s="34">
+        <f t="shared" ref="D2:D33" si="0">B2*C2</f>
         <v>0.59</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="41" t="s">
+      <c r="H2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="33" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="37">
-        <v>1</v>
-      </c>
-      <c r="C3" s="38">
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="34">
         <v>0.5</v>
       </c>
-      <c r="D3" s="43">
-        <f>B3*C3</f>
+      <c r="D3" s="39">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="37" t="s">
+      <c r="H3" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="47" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="B4" s="37">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38">
+      <c r="B4" s="33">
+        <v>1</v>
+      </c>
+      <c r="C4" s="34">
         <v>0.7</v>
       </c>
-      <c r="D4" s="38">
-        <f>B4*C4</f>
+      <c r="D4" s="34">
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="H4" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="44" t="s">
+      <c r="H4" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="61" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="33">
         <v>5</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="34">
         <v>0.14199999999999999</v>
       </c>
-      <c r="D5" s="43">
-        <f>B5*C5</f>
+      <c r="D5" s="39">
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="H5" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5" s="37" t="s">
+      <c r="H5" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="33" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="42">
         <v>5</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="43">
         <v>0.158</v>
       </c>
-      <c r="D6" s="47">
-        <f>B6*C6</f>
+      <c r="D6" s="43">
+        <f t="shared" si="0"/>
         <v>0.79</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="H6" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="46" t="s">
+      <c r="H6" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="42" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="37">
-        <v>1</v>
-      </c>
-      <c r="C7" s="38">
+      <c r="B7" s="33">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34">
         <v>2.97</v>
       </c>
-      <c r="D7" s="38">
-        <f>B7*C7</f>
+      <c r="D7" s="34">
+        <f t="shared" si="0"/>
         <v>2.97</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="35" t="s">
         <v>232</v>
       </c>
-      <c r="H7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="37" t="s">
+      <c r="H7" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="33" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="33">
         <v>5</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="34">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="D8" s="43">
-        <f>B8*C8</f>
+      <c r="D8" s="39">
+        <f t="shared" si="0"/>
         <v>0.48499999999999999</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="37" t="s">
+      <c r="H8" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="33">
         <v>3</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="34">
         <v>1.57</v>
       </c>
-      <c r="D9" s="38">
-        <f>B9*C9</f>
+      <c r="D9" s="34">
+        <f t="shared" si="0"/>
         <v>4.71</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="35" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="H9" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="37" t="s">
+      <c r="H9" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="33" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="33">
         <v>12</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="34">
         <v>0.122</v>
       </c>
-      <c r="D10" s="43">
-        <f>B10*C10</f>
+      <c r="D10" s="39">
+        <f t="shared" si="0"/>
         <v>1.464</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="37" t="s">
+      <c r="H10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="33" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="37">
-        <v>1</v>
-      </c>
-      <c r="C11" s="38">
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="34">
         <v>0.38</v>
       </c>
-      <c r="D11" s="38">
-        <f>B11*C11</f>
+      <c r="D11" s="34">
+        <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="H11" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="41" t="s">
+      <c r="H11" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="37" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="37">
-        <v>1</v>
-      </c>
-      <c r="C12" s="38">
+      <c r="B12" s="33">
+        <v>1</v>
+      </c>
+      <c r="C12" s="34">
         <v>0.38</v>
       </c>
-      <c r="D12" s="38">
-        <f>B12*C12</f>
+      <c r="D12" s="34">
+        <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="H12" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I12" s="37" t="s">
+      <c r="H12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="33" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B13" s="37">
-        <v>1</v>
-      </c>
-      <c r="C13" s="38">
+      <c r="B13" s="33">
+        <v>1</v>
+      </c>
+      <c r="C13" s="34">
         <v>0.71</v>
       </c>
-      <c r="D13" s="38">
-        <f>B13*C13</f>
+      <c r="D13" s="34">
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="H13" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="37" t="s">
+      <c r="H13" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="33" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="33">
         <v>15</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="34">
         <v>0.16600000000000001</v>
       </c>
-      <c r="D14" s="43">
-        <f>B14*C14</f>
+      <c r="D14" s="39">
+        <f t="shared" si="0"/>
         <v>2.4900000000000002</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" s="37" t="s">
+      <c r="H14" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="33">
         <v>11</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="34">
         <v>4.7E-2</v>
       </c>
-      <c r="D15" s="43">
-        <f>B15*C15</f>
+      <c r="D15" s="39">
+        <f t="shared" si="0"/>
         <v>0.51700000000000002</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="37" t="s">
+      <c r="H15" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="33">
         <f>12+11+4+3+3</f>
         <v>33</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="34">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="D16" s="43">
-        <f>B16*C16</f>
+      <c r="D16" s="39">
+        <f t="shared" si="0"/>
         <v>0.92400000000000004</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="37" t="s">
+      <c r="H16" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="33">
         <v>4</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="34">
         <v>0.20799999999999999</v>
       </c>
-      <c r="D17" s="43">
-        <f>B17*C17</f>
+      <c r="D17" s="39">
+        <f t="shared" si="0"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H17" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="37" t="s">
+      <c r="H17" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="37">
+      <c r="B18" s="33">
         <v>10</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="34">
         <v>0.191</v>
       </c>
-      <c r="D18" s="43">
-        <f>B18*C18</f>
+      <c r="D18" s="39">
+        <f t="shared" si="0"/>
         <v>1.9100000000000001</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" s="37" t="s">
+      <c r="H18" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I18" s="33" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="33">
         <v>6</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="34">
         <v>0.3</v>
       </c>
-      <c r="D19" s="38">
-        <f>B19*C19</f>
+      <c r="D19" s="34">
+        <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="H19" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" s="37" t="s">
+      <c r="H19" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="33" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="37">
-        <v>1</v>
-      </c>
-      <c r="C20" s="38">
+      <c r="B20" s="33">
+        <v>1</v>
+      </c>
+      <c r="C20" s="34">
         <v>1.04</v>
       </c>
-      <c r="D20" s="38">
-        <f>B20*C20</f>
+      <c r="D20" s="34">
+        <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="H20" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I20" s="37" t="s">
+      <c r="H20" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="33" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="37">
-        <v>1</v>
-      </c>
-      <c r="C21" s="38">
+      <c r="B21" s="33">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34">
         <v>0.45</v>
       </c>
-      <c r="D21" s="38">
-        <f>B21*C21</f>
+      <c r="D21" s="34">
+        <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" s="41" t="s">
+      <c r="H21" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="37" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="37">
+      <c r="B22" s="33">
         <f>4+2+2+3</f>
         <v>11</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="34">
         <v>0.29699999999999999</v>
       </c>
-      <c r="D22" s="43">
-        <f>B22*C22</f>
+      <c r="D22" s="39">
+        <f t="shared" si="0"/>
         <v>3.2669999999999999</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="37" t="s">
+      <c r="H22" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="33" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="37">
+      <c r="B23" s="33">
         <v>2</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="34">
         <v>1.33</v>
       </c>
-      <c r="D23" s="38">
-        <f>B23*C23</f>
+      <c r="D23" s="34">
+        <f t="shared" si="0"/>
         <v>2.66</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="H23" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="37" t="s">
+      <c r="H23" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" s="33" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="B24" s="37">
-        <v>1</v>
-      </c>
-      <c r="C24" s="38">
+      <c r="B24" s="33">
+        <v>1</v>
+      </c>
+      <c r="C24" s="34">
         <v>0.39</v>
       </c>
-      <c r="D24" s="38">
-        <f>B24*C24</f>
+      <c r="D24" s="34">
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="H24" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="37" t="s">
+      <c r="H24" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="33" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="33">
         <v>3</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="34">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D25" s="38">
-        <f>B25*C25</f>
+      <c r="D25" s="34">
+        <f t="shared" si="0"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="H25" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="37" t="s">
+      <c r="H25" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="33" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="37">
-        <v>1</v>
-      </c>
-      <c r="C26" s="38">
+      <c r="B26" s="33">
+        <v>1</v>
+      </c>
+      <c r="C26" s="34">
         <v>0.49</v>
       </c>
-      <c r="D26" s="38">
-        <f>B26*C26</f>
+      <c r="D26" s="34">
+        <f t="shared" si="0"/>
         <v>0.49</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="G26" s="39" t="s">
+      <c r="G26" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="H26" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I26" s="37" t="s">
+      <c r="H26" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="33" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="33">
         <v>5</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="34">
         <v>0.17</v>
       </c>
-      <c r="D27" s="38">
-        <f>B27*C27</f>
+      <c r="D27" s="34">
+        <f t="shared" si="0"/>
         <v>0.85000000000000009</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="35">
         <v>742792651</v>
       </c>
-      <c r="H27" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I27" s="37" t="s">
+      <c r="H27" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I27" s="33" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="33">
         <v>15</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C28" s="34">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D28" s="43">
-        <f>B28*C28</f>
+      <c r="D28" s="39">
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="H28" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="37" t="s">
+      <c r="H28" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="33">
         <v>2</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="34">
         <v>0.74</v>
       </c>
-      <c r="D29" s="38">
-        <f>B29*C29</f>
+      <c r="D29" s="34">
+        <f t="shared" si="0"/>
         <v>1.48</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="H29" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I29" s="37" t="s">
+      <c r="H29" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" s="33" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="37">
+      <c r="B30" s="33">
         <v>13</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D30" s="38">
-        <f>B30*C30</f>
+      <c r="D30" s="34">
+        <f t="shared" si="0"/>
         <v>0.12609999999999999</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="H30" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I30" s="37" t="s">
+      <c r="H30" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="37">
+      <c r="B31" s="33">
         <f>13+4+2+6+2</f>
         <v>27</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C31" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D31" s="43">
-        <f>B31*C31</f>
+      <c r="D31" s="39">
+        <f t="shared" si="0"/>
         <v>0.26190000000000002</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="37" t="s">
+      <c r="H31" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="37">
+      <c r="B32" s="33">
         <v>3</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D32" s="38">
-        <f>B32*C32</f>
+      <c r="D32" s="34">
+        <f t="shared" si="0"/>
         <v>2.9100000000000001E-2</v>
       </c>
-      <c r="E32" s="39" t="s">
+      <c r="E32" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="H32" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I32" s="37" t="s">
+      <c r="H32" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" s="33" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="37">
+      <c r="B33" s="33">
         <f>15+1+1+5</f>
         <v>22</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D33" s="43">
-        <f>B33*C33</f>
+      <c r="D33" s="39">
+        <f t="shared" si="0"/>
         <v>0.21340000000000001</v>
       </c>
-      <c r="E33" s="39" t="s">
+      <c r="E33" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G33" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I33" s="64" t="s">
+      <c r="H33" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="60" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="33">
         <f>4+1+2+2</f>
         <v>9</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D34" s="43">
-        <f>B34*C34</f>
+      <c r="D34" s="39">
+        <f t="shared" ref="D34:D65" si="1">B34*C34</f>
         <v>8.7300000000000003E-2</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I34" s="37" t="s">
+      <c r="H34" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="37">
+      <c r="B35" s="33">
         <v>4</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D35" s="38">
-        <f>B35*C35</f>
+      <c r="D35" s="34">
+        <f t="shared" si="1"/>
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="F35" s="39" t="s">
+      <c r="F35" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="39" t="s">
+      <c r="G35" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="H35" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I35" s="37" t="s">
+      <c r="H35" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="37">
-        <v>1</v>
-      </c>
-      <c r="C36" s="38">
+      <c r="B36" s="33">
+        <v>1</v>
+      </c>
+      <c r="C36" s="34">
         <v>2.4E-2</v>
       </c>
-      <c r="D36" s="38">
-        <f>B36*C36</f>
+      <c r="D36" s="34">
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
-      <c r="E36" s="39" t="s">
+      <c r="E36" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="39" t="s">
+      <c r="F36" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="G36" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="H36" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="37" t="s">
+      <c r="H36" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="37">
+      <c r="B37" s="33">
         <f>10+1+1+1</f>
         <v>13</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="34">
         <v>9.7000000000000003E-3</v>
       </c>
-      <c r="D37" s="43">
-        <f>B37*C37</f>
+      <c r="D37" s="39">
+        <f t="shared" si="1"/>
         <v>0.12609999999999999</v>
       </c>
-      <c r="E37" s="39" t="s">
+      <c r="E37" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G37" s="39" t="s">
+      <c r="G37" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I37" s="37" t="s">
+      <c r="H37" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="51">
-        <v>1</v>
-      </c>
-      <c r="C38" s="52">
+      <c r="B38" s="47">
+        <v>1</v>
+      </c>
+      <c r="C38" s="48">
         <v>0.27</v>
       </c>
-      <c r="D38" s="52">
-        <f>B38*C38</f>
+      <c r="D38" s="48">
+        <f t="shared" si="1"/>
         <v>0.27</v>
       </c>
-      <c r="E38" s="50" t="s">
+      <c r="E38" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F38" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="G38" s="50" t="s">
+      <c r="G38" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="I38" s="51" t="s">
+      <c r="H38" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" s="47" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B39" s="54">
-        <v>1</v>
-      </c>
-      <c r="C39" s="55">
+      <c r="B39" s="50">
+        <v>1</v>
+      </c>
+      <c r="C39" s="51">
         <v>2.2400000000000002</v>
       </c>
-      <c r="D39" s="55">
-        <f>B39*C39</f>
+      <c r="D39" s="51">
+        <f t="shared" si="1"/>
         <v>2.2400000000000002</v>
       </c>
-      <c r="E39" s="56" t="s">
+      <c r="E39" s="52" t="s">
         <v>268</v>
       </c>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="56" t="s">
+      <c r="G39" s="52" t="s">
         <v>268</v>
       </c>
-      <c r="H39" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I39" s="54" t="s">
+      <c r="H39" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I39" s="50" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="51">
+      <c r="B40" s="47">
         <v>5</v>
       </c>
-      <c r="C40" s="52">
+      <c r="C40" s="48">
         <v>0</v>
       </c>
-      <c r="D40" s="52">
-        <f>B40*C40</f>
+      <c r="D40" s="48">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="46" t="s">
         <v>294</v>
       </c>
-      <c r="F40" s="50" t="s">
+      <c r="F40" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="50" t="s">
+      <c r="G40" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="H40" s="51" t="s">
+      <c r="H40" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="I40" s="51" t="s">
+      <c r="I40" s="47" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="B41" s="54">
-        <v>1</v>
-      </c>
-      <c r="C41" s="55">
+      <c r="B41" s="50">
+        <v>1</v>
+      </c>
+      <c r="C41" s="51">
         <v>6.91</v>
       </c>
-      <c r="D41" s="55">
-        <f>B41*C41</f>
+      <c r="D41" s="51">
+        <f t="shared" si="1"/>
         <v>6.91</v>
       </c>
-      <c r="E41" s="56" t="s">
+      <c r="E41" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="F41" s="56" t="s">
+      <c r="F41" s="52" t="s">
         <v>242</v>
       </c>
-      <c r="G41" s="56" t="s">
+      <c r="G41" s="52" t="s">
         <v>243</v>
       </c>
-      <c r="H41" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I41" s="54" t="s">
+      <c r="H41" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="50" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="54" t="s">
         <v>272</v>
       </c>
-      <c r="B42" s="51">
-        <v>1</v>
-      </c>
-      <c r="C42" s="52">
+      <c r="B42" s="47">
+        <v>1</v>
+      </c>
+      <c r="C42" s="48">
         <v>4.78</v>
       </c>
-      <c r="D42" s="52">
-        <f>B42*C42</f>
+      <c r="D42" s="48">
+        <f t="shared" si="1"/>
         <v>4.78</v>
       </c>
-      <c r="E42" s="50" t="s">
+      <c r="E42" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="F42" s="50" t="s">
+      <c r="F42" s="46" t="s">
         <v>279</v>
       </c>
-      <c r="G42" s="50" t="s">
+      <c r="G42" s="46" t="s">
         <v>280</v>
       </c>
-      <c r="H42" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="I42" s="51" t="s">
+      <c r="H42" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" s="31" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="60">
-        <v>1</v>
-      </c>
-      <c r="C43" s="61">
+      <c r="B43" s="56">
+        <v>1</v>
+      </c>
+      <c r="C43" s="57">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D43" s="61">
-        <f>B43*C43</f>
+      <c r="D43" s="57">
+        <f t="shared" si="1"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="E43" s="62" t="s">
+      <c r="E43" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="F43" s="62" t="s">
+      <c r="F43" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="G43" s="62" t="s">
+      <c r="G43" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="H43" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I43" s="60" t="s">
+      <c r="H43" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="30" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="53" t="s">
+      <c r="A44" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="54">
-        <v>1</v>
-      </c>
-      <c r="C44" s="55">
+      <c r="B44" s="50">
+        <v>1</v>
+      </c>
+      <c r="C44" s="51">
         <v>1.7</v>
       </c>
-      <c r="D44" s="55">
-        <f>B44*C44</f>
+      <c r="D44" s="51">
+        <f t="shared" si="1"/>
         <v>1.7</v>
       </c>
-      <c r="E44" s="56" t="s">
+      <c r="E44" s="52" t="s">
         <v>269</v>
       </c>
-      <c r="F44" s="56" t="s">
+      <c r="F44" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="G44" s="56" t="s">
+      <c r="G44" s="52" t="s">
         <v>283</v>
       </c>
-      <c r="H44" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I44" s="54" t="s">
+      <c r="H44" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="50" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="B45" s="54">
-        <v>1</v>
-      </c>
-      <c r="C45" s="55">
+      <c r="B45" s="50">
+        <v>1</v>
+      </c>
+      <c r="C45" s="51">
         <v>0.35</v>
       </c>
-      <c r="D45" s="55">
-        <f>B45*C45</f>
+      <c r="D45" s="51">
+        <f t="shared" si="1"/>
         <v>0.35</v>
       </c>
-      <c r="E45" s="56" t="s">
+      <c r="E45" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="F45" s="56" t="s">
+      <c r="F45" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="G45" s="56" t="s">
+      <c r="G45" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="H45" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" s="63" t="s">
+      <c r="H45" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="59" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="54" t="s">
         <v>271</v>
       </c>
-      <c r="B46" s="51">
-        <v>1</v>
-      </c>
-      <c r="C46" s="52">
+      <c r="B46" s="47">
+        <v>1</v>
+      </c>
+      <c r="C46" s="48">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D46" s="52">
-        <f>B46*C46</f>
+      <c r="D46" s="48">
+        <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="E46" s="50" t="s">
+      <c r="E46" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="F46" s="50" t="s">
+      <c r="F46" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="G46" s="50" t="s">
+      <c r="G46" s="46" t="s">
         <v>276</v>
       </c>
-      <c r="H46" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="I46" s="51" t="s">
+      <c r="H46" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I46" s="47" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="55" t="s">
         <v>274</v>
       </c>
-      <c r="B47" s="60">
-        <v>1</v>
-      </c>
-      <c r="C47" s="61">
+      <c r="B47" s="56">
+        <v>1</v>
+      </c>
+      <c r="C47" s="57">
         <v>2.41</v>
       </c>
-      <c r="D47" s="61">
-        <f>B47*C47</f>
+      <c r="D47" s="57">
+        <f t="shared" si="1"/>
         <v>2.41</v>
       </c>
-      <c r="E47" s="62" t="s">
+      <c r="E47" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="F47" s="62" t="s">
+      <c r="F47" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="G47" s="62" t="s">
+      <c r="G47" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="H47" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I47" s="60" t="s">
+      <c r="H47" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="56" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="54">
-        <v>1</v>
-      </c>
-      <c r="C48" s="54">
+      <c r="B48" s="50">
+        <v>1</v>
+      </c>
+      <c r="C48" s="50">
         <v>4.8</v>
       </c>
-      <c r="D48" s="54">
-        <f>B48*C48</f>
+      <c r="D48" s="50">
+        <f t="shared" si="1"/>
         <v>4.8</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="56" t="s">
+      <c r="F48" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="56" t="s">
+      <c r="G48" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="H48" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I48" s="54" t="s">
-        <v>67</v>
+      <c r="H48" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="30" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="54">
-        <v>1</v>
-      </c>
-      <c r="C49" s="54">
+      <c r="B49" s="50">
+        <v>1</v>
+      </c>
+      <c r="C49" s="50">
         <v>0.59</v>
       </c>
-      <c r="D49" s="54">
-        <f>B49*C49</f>
+      <c r="D49" s="50">
+        <f t="shared" si="1"/>
         <v>0.59</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="F49" s="56" t="s">
+      <c r="F49" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G49" s="56" t="s">
+      <c r="G49" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="H49" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I49" s="54" t="s">
+      <c r="H49" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I49" s="50" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="B50" s="54">
-        <v>1</v>
-      </c>
-      <c r="C50" s="54">
+      <c r="B50" s="50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="50">
         <v>2.88</v>
       </c>
-      <c r="D50" s="54">
-        <f>B50*C50</f>
+      <c r="D50" s="50">
+        <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
-      <c r="E50" s="56" t="s">
+      <c r="E50" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="F50" s="56" t="s">
+      <c r="F50" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G50" s="56" t="s">
+      <c r="G50" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="H50" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="I50" s="54" t="s">
+      <c r="H50" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I50" s="50" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:I50">
-    <sortCondition sortBy="cellColor" ref="F2:F50" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="F2:F50" dxfId="0"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="H8" r:id="rId1"/>
@@ -3539,9 +3526,10 @@
     <hyperlink ref="H13" r:id="rId45"/>
     <hyperlink ref="H32" r:id="rId46"/>
     <hyperlink ref="H27" r:id="rId47"/>
+    <hyperlink ref="I48" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -3568,32 +3556,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -4255,10 +4243,10 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="64"/>
       <c r="E24" s="12">
         <f>SUM(E4:E22)</f>
         <v>15.232399999999998</v>
@@ -5009,10 +4997,10 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="11">
         <f>SUM(E2:E21)</f>
         <v>3.2857000000000003</v>
@@ -5622,10 +5610,10 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="33"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="11">
         <f>SUM(E2:E17)</f>
         <v>5.8091999999999997</v>
@@ -6470,10 +6458,10 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="64"/>
       <c r="E26" s="11">
         <f>SUM(E2:E24)</f>
         <v>19.491899999999998</v>
@@ -7391,10 +7379,10 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="32"/>
+      <c r="D28" s="64"/>
       <c r="E28" s="11">
         <f>SUM(E2:E26)</f>
         <v>24.016500000000001</v>

</xml_diff>

<commit_message>
Adding USB LED SubBoard 0-2
</commit_message>
<xml_diff>
--- a/REV 0-2 PCB/FlatPack 0-2/FlatPack 0-2 BOM.xlsx
+++ b/REV 0-2 PCB/FlatPack 0-2/FlatPack 0-2 BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents - HDD\Projects\FusIon-Pack\REV 0-2 PCB\FlatPack 0-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\FusIon-Pack\REV 0-2 PCB\FlatPack 0-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD2DC70-694F-4705-9460-5BF8D49E2A2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete BOM" sheetId="6" r:id="rId1"/>
@@ -22,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Button-Interface SubBoard 0-2'!$A$1:$J$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -942,7 +943,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1939,11 +1940,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2974,7 +2975,7 @@
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="D34" s="39">
-        <f t="shared" ref="D34:D65" si="1">B34*C34</f>
+        <f t="shared" ref="D34:D50" si="1">B34*C34</f>
         <v>8.7300000000000003E-2</v>
       </c>
       <c r="E34" s="35" t="s">
@@ -3479,54 +3480,54 @@
     <sortCondition sortBy="cellColor" ref="F2:F50" dxfId="0"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H14" r:id="rId2"/>
-    <hyperlink ref="H48" r:id="rId3"/>
-    <hyperlink ref="H38" r:id="rId4"/>
-    <hyperlink ref="H37" r:id="rId5"/>
-    <hyperlink ref="H33" r:id="rId6"/>
-    <hyperlink ref="H34" r:id="rId7"/>
-    <hyperlink ref="H31" r:id="rId8"/>
-    <hyperlink ref="H18" r:id="rId9"/>
-    <hyperlink ref="H3" r:id="rId10"/>
-    <hyperlink ref="H28" r:id="rId11"/>
-    <hyperlink ref="H16" r:id="rId12"/>
-    <hyperlink ref="H22" r:id="rId13"/>
-    <hyperlink ref="H5" r:id="rId14"/>
-    <hyperlink ref="H10" r:id="rId15"/>
-    <hyperlink ref="H30" r:id="rId16"/>
-    <hyperlink ref="H36" r:id="rId17"/>
-    <hyperlink ref="H26" r:id="rId18"/>
-    <hyperlink ref="H43" r:id="rId19"/>
-    <hyperlink ref="I43" r:id="rId20"/>
-    <hyperlink ref="H4" r:id="rId21"/>
-    <hyperlink ref="H11" r:id="rId22"/>
-    <hyperlink ref="H12" r:id="rId23"/>
-    <hyperlink ref="H50" r:id="rId24"/>
-    <hyperlink ref="H21" r:id="rId25"/>
-    <hyperlink ref="H45" r:id="rId26"/>
-    <hyperlink ref="H2" r:id="rId27"/>
-    <hyperlink ref="H35" r:id="rId28"/>
-    <hyperlink ref="H6" r:id="rId29"/>
-    <hyperlink ref="H23" r:id="rId30"/>
-    <hyperlink ref="H25" r:id="rId31"/>
-    <hyperlink ref="H20" r:id="rId32"/>
-    <hyperlink ref="H7" r:id="rId33"/>
-    <hyperlink ref="H24" r:id="rId34"/>
-    <hyperlink ref="H19" r:id="rId35"/>
-    <hyperlink ref="H29" r:id="rId36"/>
-    <hyperlink ref="H49" r:id="rId37"/>
-    <hyperlink ref="H41" r:id="rId38"/>
-    <hyperlink ref="H46" r:id="rId39"/>
-    <hyperlink ref="H42" r:id="rId40"/>
-    <hyperlink ref="I42" r:id="rId41"/>
-    <hyperlink ref="H39" r:id="rId42"/>
-    <hyperlink ref="H44" r:id="rId43"/>
-    <hyperlink ref="H9" r:id="rId44"/>
-    <hyperlink ref="H13" r:id="rId45"/>
-    <hyperlink ref="H32" r:id="rId46"/>
-    <hyperlink ref="H27" r:id="rId47"/>
-    <hyperlink ref="I48" r:id="rId48"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H48" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H38" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H37" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H34" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H31" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H28" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H30" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H36" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H43" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I43" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H4" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H11" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H12" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H50" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H21" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H45" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H2" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H35" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H6" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H23" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H25" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H20" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H7" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H24" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H29" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H49" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H46" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="I42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H9" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H13" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H32" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H27" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="I48" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId49"/>
@@ -3534,7 +3535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -4259,23 +4260,23 @@
     <mergeCell ref="C24:D24"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I11" r:id="rId1"/>
-    <hyperlink ref="I15" r:id="rId2"/>
-    <hyperlink ref="I22" r:id="rId3"/>
-    <hyperlink ref="I21" r:id="rId4"/>
-    <hyperlink ref="I16" r:id="rId5"/>
-    <hyperlink ref="I18" r:id="rId6"/>
-    <hyperlink ref="I20" r:id="rId7"/>
-    <hyperlink ref="I19" r:id="rId8"/>
-    <hyperlink ref="I17" r:id="rId9"/>
-    <hyperlink ref="I12" r:id="rId10"/>
-    <hyperlink ref="I9" r:id="rId11"/>
-    <hyperlink ref="I4" r:id="rId12"/>
-    <hyperlink ref="I5" r:id="rId13"/>
-    <hyperlink ref="I6" r:id="rId14"/>
-    <hyperlink ref="I7" r:id="rId15"/>
-    <hyperlink ref="I8" r:id="rId16"/>
-    <hyperlink ref="I10" r:id="rId17"/>
+    <hyperlink ref="I11" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I22" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I21" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I16" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I18" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I20" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I19" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I17" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I12" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I9" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I4" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I5" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I6" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I7" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I8" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="I10" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>
@@ -4283,11 +4284,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5011,22 +5012,22 @@
     <mergeCell ref="C23:D23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I7" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I13" r:id="rId5"/>
-    <hyperlink ref="I14" r:id="rId6"/>
-    <hyperlink ref="I15" r:id="rId7"/>
-    <hyperlink ref="I16" r:id="rId8"/>
-    <hyperlink ref="I18" r:id="rId9"/>
-    <hyperlink ref="I17" r:id="rId10"/>
-    <hyperlink ref="I19" r:id="rId11"/>
-    <hyperlink ref="I20" r:id="rId12"/>
-    <hyperlink ref="J20" r:id="rId13"/>
-    <hyperlink ref="I21" r:id="rId14"/>
-    <hyperlink ref="I4" r:id="rId15"/>
-    <hyperlink ref="I6" r:id="rId16"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="I13" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I14" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="I15" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="I16" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="I18" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="I17" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="I19" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="I20" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J20" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="I21" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="I4" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="I6" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -5034,7 +5035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5624,20 +5625,20 @@
     <mergeCell ref="C19:D19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I14" r:id="rId1"/>
-    <hyperlink ref="I13" r:id="rId2"/>
-    <hyperlink ref="I11" r:id="rId3"/>
-    <hyperlink ref="I2" r:id="rId4"/>
-    <hyperlink ref="I3" r:id="rId5"/>
-    <hyperlink ref="I4" r:id="rId6"/>
-    <hyperlink ref="I6" r:id="rId7"/>
-    <hyperlink ref="I7" r:id="rId8"/>
-    <hyperlink ref="I16" r:id="rId9"/>
-    <hyperlink ref="I10" r:id="rId10"/>
-    <hyperlink ref="I5" r:id="rId11"/>
-    <hyperlink ref="I15" r:id="rId12"/>
-    <hyperlink ref="I17" r:id="rId13"/>
-    <hyperlink ref="I12" r:id="rId14"/>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I13" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I11" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I3" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I4" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I7" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="I16" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="I10" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="I5" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="I17" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="I12" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>
@@ -5645,11 +5646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="B2:J24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6472,27 +6473,27 @@
     <mergeCell ref="C26:D26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I6" r:id="rId4"/>
-    <hyperlink ref="I7" r:id="rId5"/>
-    <hyperlink ref="I8" r:id="rId6"/>
-    <hyperlink ref="I13" r:id="rId7"/>
-    <hyperlink ref="I16" r:id="rId8"/>
-    <hyperlink ref="I18" r:id="rId9"/>
-    <hyperlink ref="I20" r:id="rId10"/>
-    <hyperlink ref="I21" r:id="rId11"/>
-    <hyperlink ref="I22" r:id="rId12"/>
-    <hyperlink ref="I15" r:id="rId13"/>
-    <hyperlink ref="I14" r:id="rId14"/>
-    <hyperlink ref="I12" r:id="rId15"/>
-    <hyperlink ref="I5" r:id="rId16"/>
-    <hyperlink ref="I9" r:id="rId17"/>
-    <hyperlink ref="I17" r:id="rId18"/>
-    <hyperlink ref="I19" r:id="rId19"/>
-    <hyperlink ref="I23" r:id="rId20"/>
-    <hyperlink ref="I24" r:id="rId21"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="I13" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="I16" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="I18" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="I20" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="I21" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="I22" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="I15" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="I14" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="I12" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="I5" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="I9" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="I17" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="I19" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="I23" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="I24" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
@@ -6500,10 +6501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J26"/>
     </sheetView>
   </sheetViews>
@@ -7393,29 +7394,29 @@
     <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I8" r:id="rId6"/>
-    <hyperlink ref="I14" r:id="rId7"/>
-    <hyperlink ref="I15" r:id="rId8"/>
-    <hyperlink ref="I17" r:id="rId9"/>
-    <hyperlink ref="I19" r:id="rId10"/>
-    <hyperlink ref="I20" r:id="rId11"/>
-    <hyperlink ref="I21" r:id="rId12"/>
-    <hyperlink ref="I23" r:id="rId13"/>
-    <hyperlink ref="I7" r:id="rId14"/>
-    <hyperlink ref="I26" r:id="rId15"/>
-    <hyperlink ref="I9" r:id="rId16"/>
-    <hyperlink ref="J9" r:id="rId17"/>
-    <hyperlink ref="I24" r:id="rId18"/>
-    <hyperlink ref="I25" r:id="rId19"/>
-    <hyperlink ref="I16" r:id="rId20"/>
-    <hyperlink ref="I18" r:id="rId21"/>
-    <hyperlink ref="I22" r:id="rId22"/>
-    <hyperlink ref="I10" r:id="rId23"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="I14" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="I15" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="I17" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="I19" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="I20" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="I21" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="I23" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="I7" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="I26" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="I9" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="J9" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="I24" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="I25" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="I16" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
+    <hyperlink ref="I18" r:id="rId21" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
+    <hyperlink ref="I22" r:id="rId22" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
+    <hyperlink ref="I10" r:id="rId23" xr:uid="{00000000-0004-0000-0500-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>